<commit_message>
Updated table structure again
</commit_message>
<xml_diff>
--- a/Table Structure.xlsx
+++ b/Table Structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTD\WPL\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTD\WPL\Project\MeanApp3\Craigslist-One\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>User</t>
   </si>
@@ -137,9 +137,6 @@
     <t>DateAvaiable</t>
   </si>
   <si>
-    <t>TypeId</t>
-  </si>
-  <si>
     <t>Furnished</t>
   </si>
   <si>
@@ -150,12 +147,6 @@
   </si>
   <si>
     <t>CatId</t>
-  </si>
-  <si>
-    <t>HouseType</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>Condition</t>
@@ -571,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Z31"/>
+  <dimension ref="A3:Y28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J9" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,31 +579,31 @@
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -662,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -697,7 +688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -725,9 +716,8 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -797,23 +787,20 @@
       <c r="W19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X19" s="4" t="s">
+      <c r="X19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Y19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Z19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -821,50 +808,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>